<commit_message>
Se incluye función de flexión para HSS
</commit_message>
<xml_diff>
--- a/estructura de modulo y funciones python.xlsx
+++ b/estructura de modulo y funciones python.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\3.Desarrollo\5.Codigos_phyton\01-Memorias_calculo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\3.Desarrollo\5.Codigos_phyton\01-Memorias_calculo\desarrollo_estructuras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103E77E4-0A5C-405F-ADC5-0FD8B11FDC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BD2ECA-F188-4088-A347-B570EF6B877C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{510EE5EC-72F8-45C3-8FA3-75253294C02F}"/>
+    <workbookView xWindow="7305" yWindow="1950" windowWidth="12000" windowHeight="7995" xr2:uid="{510EE5EC-72F8-45C3-8FA3-75253294C02F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="98">
   <si>
     <t>prop_mat</t>
   </si>
@@ -132,9 +132,6 @@
     <t>ARGUMENTS</t>
   </si>
   <si>
-    <t>stren_flex_yield</t>
-  </si>
-  <si>
     <t>Flexural strength for yielding-Plastic moment</t>
   </si>
   <si>
@@ -168,24 +165,9 @@
     <t>TABLE B4.1b</t>
   </si>
   <si>
-    <t>F2.1</t>
-  </si>
-  <si>
     <t>Lateral torsional buckling for compact-compact section</t>
   </si>
   <si>
-    <t>F2.2</t>
-  </si>
-  <si>
-    <t>stren_flex_c_c_ltb</t>
-  </si>
-  <si>
-    <t>stren_flex_ncs_c_flb</t>
-  </si>
-  <si>
-    <t>F2.3</t>
-  </si>
-  <si>
     <t>slend_i_s</t>
   </si>
   <si>
@@ -196,6 +178,159 @@
   </si>
   <si>
     <t>TABLE D1.1a</t>
+  </si>
+  <si>
+    <t>Compression flange local buckling for noncompact/slender-compact section</t>
+  </si>
+  <si>
+    <t>Compression flange yielding for compact/noncompact/slender-noncompact section</t>
+  </si>
+  <si>
+    <t>Lateral torsional buckling for compact/noncompact/slender-noncompact section</t>
+  </si>
+  <si>
+    <t>SECTION F2.1</t>
+  </si>
+  <si>
+    <t>SECTION F2.2</t>
+  </si>
+  <si>
+    <t>SUB-CATEGORY</t>
+  </si>
+  <si>
+    <t>PROFILE TYPE</t>
+  </si>
+  <si>
+    <t>SECTION F3.2</t>
+  </si>
+  <si>
+    <t>SECTION F4.1</t>
+  </si>
+  <si>
+    <t>SECTION F4.2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>compression</t>
+  </si>
+  <si>
+    <t>flexure</t>
+  </si>
+  <si>
+    <t>n.a.</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>hss rectangular</t>
+  </si>
+  <si>
+    <t>hss circular</t>
+  </si>
+  <si>
+    <t>angular</t>
+  </si>
+  <si>
+    <t>stren_flex_i_y_F2_1</t>
+  </si>
+  <si>
+    <t>stren_flex_i_ltb_F2_2</t>
+  </si>
+  <si>
+    <t>stren_flex_i_flb_F3_2</t>
+  </si>
+  <si>
+    <t>stren_flex_i_cfy_F4_1</t>
+  </si>
+  <si>
+    <t>stren_flex_i_ltb_F4_2</t>
+  </si>
+  <si>
+    <t>stren_flex_i_ltb_F4_3</t>
+  </si>
+  <si>
+    <t>SECTION F4.3</t>
+  </si>
+  <si>
+    <t>Compression flange local buckling for compact/noncompact/slender-noncompact section</t>
+  </si>
+  <si>
+    <t>stren_flex_i_cfy_F5_1</t>
+  </si>
+  <si>
+    <t>SECTION F5.1</t>
+  </si>
+  <si>
+    <t>SECTION F5.2</t>
+  </si>
+  <si>
+    <t>stren_flex_i_ltb_F5_2</t>
+  </si>
+  <si>
+    <t>SECTION F5.3</t>
+  </si>
+  <si>
+    <t>stren_flex_i_flb_F5_3</t>
+  </si>
+  <si>
+    <t>stren_flex_i</t>
+  </si>
+  <si>
+    <t>Flexural strength</t>
+  </si>
+  <si>
+    <t>SECTION F</t>
+  </si>
+  <si>
+    <t>stren_flex_hss_rect</t>
+  </si>
+  <si>
+    <t>SECTION F7.1</t>
+  </si>
+  <si>
+    <t>slend_hss_rect_flex_ns</t>
+  </si>
+  <si>
+    <t>Local buckling for rectangular HSS sections in flexure - non seismic applications</t>
+  </si>
+  <si>
+    <t>stren_flex_hss_rect_y_F7_1</t>
+  </si>
+  <si>
+    <t>stren_flex_hss_rect_flb_F7_2</t>
+  </si>
+  <si>
+    <t>Flange local buckling for HSS section</t>
+  </si>
+  <si>
+    <t>SECTION F7.2</t>
+  </si>
+  <si>
+    <t>stren_flex_hss_rect_wlb_F7_3</t>
+  </si>
+  <si>
+    <t>Web local buckling for HSS section</t>
+  </si>
+  <si>
+    <t>SECTION F7.3</t>
+  </si>
+  <si>
+    <t>stren_flex_hss_rect_ltb_F7_4</t>
+  </si>
+  <si>
+    <t>Lateral torsional buckling for HSS section</t>
+  </si>
+  <si>
+    <t>SECTION F7.4</t>
+  </si>
+  <si>
+    <t>Flexural strength for HSS section</t>
+  </si>
+  <si>
+    <t>SECTION F7</t>
   </si>
 </sst>
 </file>
@@ -219,7 +354,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,12 +376,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,12 +465,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -359,11 +491,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8965DA93-5C2D-4D0E-92AC-D0B15AFC77D8}" name="Tabla1" displayName="Tabla1" ref="B2:G21" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B2:G21" xr:uid="{8965DA93-5C2D-4D0E-92AC-D0B15AFC77D8}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8965DA93-5C2D-4D0E-92AC-D0B15AFC77D8}" name="Tabla1" displayName="Tabla1" ref="B2:I33" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B2:I33" xr:uid="{8965DA93-5C2D-4D0E-92AC-D0B15AFC77D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I23">
+    <sortCondition ref="C2:C23"/>
+  </sortState>
+  <tableColumns count="8">
     <tableColumn id="4" xr3:uid="{D41B88B0-8D9C-4C3C-B393-16F5BE4BBD35}" name="MÓDULO"/>
     <tableColumn id="5" xr3:uid="{6FD665D2-7E97-4E19-B320-4AC51E81D46B}" name="CATEGORY"/>
+    <tableColumn id="2" xr3:uid="{EE26195A-337E-4DD3-ABE8-228A04008EE0}" name="SUB-CATEGORY"/>
+    <tableColumn id="7" xr3:uid="{EB943E16-78AC-4BEA-908F-55010703EB2E}" name="PROFILE TYPE" dataDxfId="0"/>
     <tableColumn id="1" xr3:uid="{90ED8C57-2E53-48EF-8A55-9AA028D9D2FC}" name="FUNCTION-SHORT NAME"/>
     <tableColumn id="3" xr3:uid="{1B6401F1-88AD-43E5-A380-2938936FA86B}" name="DESCRIPTION"/>
     <tableColumn id="9" xr3:uid="{CEC30896-4888-4F31-9C38-8D70DB63CDCF}" name="SPECIFICATION"/>
@@ -690,22 +827,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE6627F-0394-4D34-B2EA-9C4F964D5517}">
-  <dimension ref="B2:G21"/>
+  <dimension ref="B2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="76.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
@@ -713,312 +853,756 @@
         <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" t="s">
         <v>14</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" t="s">
         <v>28</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="11" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="H19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" t="s">
         <v>47</v>
       </c>
-      <c r="E19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="4" t="s">
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
         <v>49</v>
       </c>
-      <c r="E20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
+      <c r="H23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" t="s">
+        <v>91</v>
+      </c>
+      <c r="H31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" t="s">
+        <v>94</v>
+      </c>
+      <c r="H32" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" t="s">
+        <v>39</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>